<commit_message>
Projects | Print Projects | Change in the import from Excel
</commit_message>
<xml_diff>
--- a/static/images/hotwire_template.xlsx
+++ b/static/images/hotwire_template.xlsx
@@ -38,9 +38,6 @@
     <t>CONTACT INFO</t>
   </si>
   <si>
-    <t>PROPERTY</t>
-  </si>
-  <si>
     <t>REQUEST</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>MLITAR TIME (HH:MM)</t>
+  </si>
+  <si>
+    <t>PROJECT ID</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G12"/>
+      <selection activeCell="A2" sqref="A2:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,19 +443,19 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="10"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="5"/>
       <c r="D3" s="9"/>
       <c r="E3" s="7"/>

</xml_diff>